<commit_message>
Added downstream coalesce data.
</commit_message>
<xml_diff>
--- a/test/fixture/snapshot/cli/sort-format/basic/commander/commander-common.xlsx
+++ b/test/fixture/snapshot/cli/sort-format/basic/commander/commander-common.xlsx
@@ -224,7 +224,7 @@
     <comment ref="C4" authorId="0">
       <text>
         <r>
-          <t>Group: decks</t>
+          <t>Group: external</t>
         </r>
       </text>
     </comment>
@@ -718,7 +718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6F1F6"/>
+        <fgColor rgb="FFE3D8F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -790,10 +790,10 @@
         <color rgb="FF999999"/>
       </right>
       <top style="thin">
-        <color rgb="FF4FA3B8"/>
+        <color rgb="FF8A6BB8"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF4FA3B8"/>
+        <color rgb="FF8A6BB8"/>
       </bottom>
       <diagonal/>
     </border>

</xml_diff>